<commit_message>
expand data type 02
</commit_message>
<xml_diff>
--- a/corpRch_ecoAct/data/ecoAct/취업자_경제활동인구_계절조정_수정.xlsx
+++ b/corpRch_ecoAct/data/ecoAct/취업자_경제활동인구_계절조정_수정.xlsx
@@ -29,7 +29,7 @@
     <t xml:space="preserve">경제활동인구</t>
   </si>
   <si>
-    <t xml:space="preserve">  취업자</t>
+    <t xml:space="preserve">취업자</t>
   </si>
   <si>
     <t xml:space="preserve">비임금근로자</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">임시근로자</t>
   </si>
   <si>
-    <t xml:space="preserve"> 일용근로자</t>
+    <t xml:space="preserve">일용근로자</t>
   </si>
   <si>
     <t xml:space="preserve">남자</t>
@@ -2893,10 +2893,10 @@
   <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="1" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="929" style="0" width="11.52"/>
@@ -12547,7 +12547,7 @@
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="158.86"/>
   </cols>

</xml_diff>